<commit_message>
bo sung release note
</commit_message>
<xml_diff>
--- a/Docs/SSI - Super Core- Deployment Guide - HNXTPRL - 20240722.xlsx
+++ b/Docs/SSI - Super Core- Deployment Guide - HNXTPRL - 20240722.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="550"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="550" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Deployment plan" sheetId="17" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="85">
   <si>
     <t>PROJECT IDENTIFICATION</t>
   </si>
@@ -387,6 +387,9 @@
 '- "EnableSaveDB": false  tắt sử dụng ghi Database
 '- "EnableSaveDB": true  bật sử dụng ghi Database
 </t>
+  </si>
+  <si>
+    <t>/ConfigApp/appsettings.json</t>
   </si>
 </sst>
 </file>
@@ -842,12 +845,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
     </xf>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -864,12 +882,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="10" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -880,15 +892,6 @@
     </xf>
     <xf numFmtId="15" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2145,7 +2148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2155,7 +2158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
@@ -2166,62 +2169,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18">
-      <c r="A1" s="42"/>
-      <c r="B1" s="43"/>
+      <c r="A1" s="47"/>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="50"/>
     </row>
     <row r="3" spans="1:2" ht="18.75" thickBot="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="44" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
     </row>
     <row r="8" spans="1:2" ht="29.25" customHeight="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
     </row>
     <row r="10" spans="1:2" ht="55.5" customHeight="1">
-      <c r="A10" s="51"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="53"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="52"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="43"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="14" t="s">
@@ -2240,82 +2243,82 @@
       <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:2" ht="27" customHeight="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1">
       <c r="A17" s="21"/>
     </row>
     <row r="18" spans="1:2" ht="18">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
     </row>
     <row r="19" spans="1:2" ht="18" customHeight="1">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="45"/>
+      <c r="B19" s="50"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" thickBot="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="41" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="43"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="53" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A24" s="49"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="43"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="43"/>
     </row>
     <row r="27" spans="1:2" ht="41.25" customHeight="1">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="41" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="43"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="44" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -2323,40 +2326,40 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="54"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="54"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A32" s="49"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1">
       <c r="A33" s="21"/>
     </row>
     <row r="34" spans="1:2" ht="18">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
     </row>
     <row r="35" spans="1:2" ht="18" customHeight="1">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="50"/>
     </row>
     <row r="36" spans="1:2" ht="18.75" thickBot="1">
-      <c r="A36" s="46"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="18" t="s">
@@ -2364,29 +2367,29 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="54"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="18" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="54"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="54"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A41" s="49"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="22"/>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="18" t="s">
@@ -2394,35 +2397,35 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="54"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="54"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="54"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="54"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A47" s="49"/>
+      <c r="A47" s="45"/>
       <c r="B47" s="22"/>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="44" t="s">
         <v>18</v>
       </c>
       <c r="B48" s="18" t="s">
@@ -2430,26 +2433,26 @@
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="54"/>
+      <c r="A49" s="46"/>
       <c r="B49" s="18" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="54"/>
+      <c r="A50" s="46"/>
       <c r="B50" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A51" s="49"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="22"/>
     </row>
     <row r="52" spans="1:2" ht="54.75" customHeight="1">
       <c r="A52" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="41" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2457,11 +2460,11 @@
       <c r="A53" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="53"/>
+      <c r="B53" s="42"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1">
       <c r="A54" s="15"/>
-      <c r="B54" s="41"/>
+      <c r="B54" s="43"/>
     </row>
     <row r="55" spans="1:2" ht="15.75" thickBot="1">
       <c r="A55" s="21"/>
@@ -2620,18 +2623,13 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A8:A9"/>
@@ -2645,13 +2643,18 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="A48:A51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2741,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2834,10 +2837,12 @@
       <c r="D4" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="37" t="s">
+        <v>84</v>
+      </c>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
-      <c r="H4" s="55" t="s">
+      <c r="H4" s="40" t="s">
         <v>83</v>
       </c>
       <c r="I4" s="36"/>

</xml_diff>